<commit_message>
Attempting to make a dataframe
</commit_message>
<xml_diff>
--- a/MyEmployeeHashTable.xlsx
+++ b/MyEmployeeHashTable.xlsx
@@ -1,66 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0D5D34-F151-41B4-ABED-E152C756BB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="AllData" sheetId="1" r:id="rId1"/>
+    <sheet name="AllData" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>b'\xaedB\x8b\x13\xeaa\xa6\x05p\xf9\x1b\xd8\xe9D\x85\xad\xa0\x95\x10\xfd\x95\xd0\xe7&gt;/\xde\xcdJ&gt;&gt;+\xa2\x88`X\xd0N\xa3\xca\x04P\xcf!\xe1w0$Ei\x93\xc2\xef&lt;\x935\xcb\xb6\xf7\x11\xdd0\xd6\xc4\x1a\x01\xd7\xef\xe2A\\\xa3\x19i\x9a\xa1\xc75M\xa2_\xbcAZj\x1e&gt;~\x9e\x0fn}\xc4\x91*\xac\xc3\xect\xe1\x0f&lt;\xd4\x06\xf3&gt;W\xf2\x7f\xcf\xe1\xa4\r\xbe\x82\x9b\x88\xa2,\xf1rp\x0c\xdf\xb1\x08y\xc2'</t>
-  </si>
-  <si>
-    <t>Baker</t>
-  </si>
-  <si>
-    <t>Janet</t>
-  </si>
-  <si>
-    <t>423456</t>
-  </si>
-  <si>
-    <t>26Jan1988</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -91,27 +66,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -158,7 +124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,27 +156,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,24 +190,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,47 +365,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>b'\xaedB\x8b\x13\xeaa\xa6\x05p\xf9\x1b\xd8\xe9D\x85\xad\xa0\x95\x10\xfd\x95\xd0\xe7&gt;/\xde\xcdJ&gt;&gt;+\xa2\x88`X\xd0N\xa3\xca\x04P\xcf!\xe1w0$Ei\x93\xc2\xef&lt;\x935\xcb\xb6\xf7\x11\xdd0\xd6\xc4\x1a\x01\xd7\xef\xe2A\\\xa3\x19i\x9a\xa1\xc75M\xa2_\xbcAZj\x1e&gt;~\x9e\x0fn}\xc4\x91*\xac\xc3\xect\xe1\x0f&lt;\xd4\x06\xf3&gt;W\xf2\x7f\xcf\xe1\xa4\r\xbe\x82\x9b\x88\xa2,\xf1rp\x0c\xdf\xb1\x08y\xc2'</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Tyler</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Kathy</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>42544</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>45645343</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Hashing and Salt
</commit_message>
<xml_diff>
--- a/MyEmployeeHashTable.xlsx
+++ b/MyEmployeeHashTable.xlsx
@@ -1,54 +1,144 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119F8456-C5C0-46B3-B2F2-D06F714391B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11160" windowWidth="20730" xWindow="-20610" yWindow="-120"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+  <si>
+    <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Tonya</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>13Apr1988</t>
+  </si>
+  <si>
+    <t>9eac806b76bab0185444c731f3f419fe67f52bc777431faba5e671097528abd3</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Janice</t>
+  </si>
+  <si>
+    <t>223456</t>
+  </si>
+  <si>
+    <t>21Jan1982</t>
+  </si>
+  <si>
+    <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:b8115ca23ae148d2b6a0cb607d3cc3f5</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>523456</t>
+  </si>
+  <si>
+    <t>12May2012</t>
+  </si>
+  <si>
+    <t>1f5ce984534afce73537d6b26f1aff3696e08da180835c45ba67654edd6054ef:b2c6b18736f84020abb055d3800fb5be</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>823546</t>
+  </si>
+  <si>
+    <t>21Dec1977</t>
+  </si>
+  <si>
+    <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:3d7cad0d00984768b3accd80a1a65e43</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>956874</t>
+  </si>
+  <si>
+    <t>15May1972</t>
+  </si>
+  <si>
+    <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:7a140436452545f384388529c6997b9f</t>
+  </si>
+  <si>
+    <t>635421</t>
+  </si>
+  <si>
+    <t>17Dec1988</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,38 +198,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -463,205 +570,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="101.7109375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="20.140625"/>
-    <col customWidth="1" max="3" min="3" style="1" width="17.28515625"/>
-    <col customWidth="1" max="4" min="4" style="1" width="19.7109375"/>
-    <col customWidth="1" max="5" min="5" style="1" width="28.5703125"/>
-    <col customWidth="1" max="8" min="6" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="9" style="1" width="9.140625"/>
+    <col min="1" max="1" width="101.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="2" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="2">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Tonya</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>13Apr1988</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>9eac806b76bab0185444c731f3f419fe67f52bc777431faba5e671097528abd3</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Anderson</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Janice</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>223456</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>21Jan1982</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:b8115ca23ae148d2b6a0cb607d3cc3f5</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Juan</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>523456</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12May2012</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>1f5ce984534afce73537d6b26f1aff3696e08da180835c45ba67654edd6054ef:b2c6b18736f84020abb055d3800fb5be</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Monroe</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>823546</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>21Dec1977</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:3d7cad0d00984768b3accd80a1a65e43</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ashley</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>956874</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>15May1972</t>
-        </is>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1:7a140436452545f384388529c6997b9f</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Smith</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>635421</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>17Dec1988</t>
-        </is>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding data retrieval to program
</commit_message>
<xml_diff>
--- a/MyEmployeeHashTable.xlsx
+++ b/MyEmployeeHashTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119F8456-C5C0-46B3-B2F2-D06F714391B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69F208-7003-40A1-B45A-8438C001B1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>9f542590100424c92a6ae40860f7017ac5dfbcff3cb49b36eace29b068e0d8e1</t>
   </si>
@@ -98,13 +98,73 @@
   </si>
   <si>
     <t>17Dec1988</t>
+  </si>
+  <si>
+    <t>c43139196d576427b9073922c4da86ff6d0ecff71d1a2c2ad9116ad2a1e8d50d:c19d2c95c02c473eac502974623d38ee</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>654217</t>
+  </si>
+  <si>
+    <t>04Mar1992</t>
+  </si>
+  <si>
+    <t>Key: 358a31529c144ab04a2712808d9e561f78e09868c535f90f653df3e0fc9a7ef1:729b0bcf3cb244229c9fca72f4c7affc</t>
+  </si>
+  <si>
+    <t>Barnhardt</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>698574</t>
+  </si>
+  <si>
+    <t>21May2019</t>
+  </si>
+  <si>
+    <t>Key: 2a214699ad186d32cfacee05b795d4fa5988439ea615acd3957922de7f1afb9c:4cc121820bc44e7e8cd03c1aabe0b714</t>
+  </si>
+  <si>
+    <t>Caldwell</t>
+  </si>
+  <si>
+    <t>Lillith</t>
+  </si>
+  <si>
+    <t>471258</t>
+  </si>
+  <si>
+    <t>06Jun2001</t>
+  </si>
+  <si>
+    <t>Key: 8a37263f023c728ad113b8a44701cd1077b7bd00724109862e875b99102e9810:c3b15fde71af4457b95248493be7a2b9</t>
+  </si>
+  <si>
+    <t>Macalilly</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>965842</t>
+  </si>
+  <si>
+    <t>17May1996</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +195,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -212,11 +282,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -231,6 +331,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -571,21 +680,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="104.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" style="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -704,6 +813,74 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Set up the ability to retrieve information.
</commit_message>
<xml_diff>
--- a/MyEmployeeHashTable.xlsx
+++ b/MyEmployeeHashTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C69F208-7003-40A1-B45A-8438C001B1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B23E79-846B-4B03-B307-2F3CACD29318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,16 +179,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -316,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,13 +323,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -683,7 +670,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +801,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
@@ -831,7 +818,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
@@ -848,7 +835,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
@@ -865,7 +852,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B11" t="s">

</xml_diff>

<commit_message>
The deletion from the excel file works, but needs cleaned up.
</commit_message>
<xml_diff>
--- a/MyEmployeeHashTable.xlsx
+++ b/MyEmployeeHashTable.xlsx
@@ -1,71 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F7642-91F5-478A-8DFD-BE0ED0AB8943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>c88ace207c628d4a1d78221c20189eaff091940592141fecb9431cf266a178b7:2857859b20e047739a787c7385b02248</t>
-  </si>
-  <si>
-    <t>0550f26c152a53f6d21c31565424edcd05db02e0cefa28e2a1d3f752234aed3c:4b4ba073b0ef4165aef48f0240359805</t>
-  </si>
-  <si>
-    <t>af6ca80fd611c30a1765fed225caf27bac2d5994dda34ab0a10acae6260e4b0c:e9c7eb9b074c40b5a5f7ac34b6fcdbd3</t>
-  </si>
-  <si>
-    <t>jfkd;ajf</t>
-  </si>
-  <si>
-    <t>reqwrew</t>
-  </si>
-  <si>
-    <t>kfjd;ajf</t>
-  </si>
-  <si>
-    <t>jfdkafj;</t>
-  </si>
-  <si>
-    <t>reqwrewqr</t>
-  </si>
-  <si>
-    <t>kfjda;sjfsdja</t>
-  </si>
-  <si>
-    <t>fkda;jksdjf</t>
-  </si>
-  <si>
-    <t>rewqrewqrewrq</t>
-  </si>
-  <si>
-    <t>kfjda;sjf;kdsjfa</t>
-  </si>
-  <si>
-    <t>fdjkaf;jdsafjdsajf;</t>
-  </si>
-  <si>
-    <t>reqwrweqr</t>
-  </si>
-  <si>
-    <t>8979</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Unnamed: 1</t>
+  </si>
+  <si>
+    <t>Unnamed: 2</t>
+  </si>
+  <si>
+    <t>Unnamed: 3</t>
+  </si>
+  <si>
+    <t>Unnamed: 4</t>
+  </si>
+  <si>
+    <t>2d0f4fde560a87908cb87b7a0a29cebd00c9f7fd38d08dbedb41ce22dd7ad879:bfb76a73f68f4327afdf0b201caf51a2</t>
+  </si>
+  <si>
+    <t>30cd31772a084fc1a31447c7e845aa4b1828ad34091d74393ff6277a66c316f7:18bc1c39b86c43e2825353c3b05c5f9a</t>
+  </si>
+  <si>
+    <t>hlkhljkhl</t>
+  </si>
+  <si>
+    <t>tuituit</t>
+  </si>
+  <si>
+    <t>hjklhljh</t>
+  </si>
+  <si>
+    <t>tuiti</t>
+  </si>
+  <si>
+    <t>jhlkh</t>
+  </si>
+  <si>
+    <t>tuiutiutiti</t>
+  </si>
+  <si>
+    <t>hjklkhhhlklh</t>
+  </si>
+  <si>
+    <t>tuit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +131,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +269,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,68 +462,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>